<commit_message>
Task: Completed daily operations, 8 hours, 09/14
</commit_message>
<xml_diff>
--- a/CISC 4900 - Time Log Spreadsheet.xlsx
+++ b/CISC 4900 - Time Log Spreadsheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicole/Desktop/FALL 2023/CISC 4900 - Independent Group:Study - Chuang:Lapid/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicole/Documents/GitHub/CISC4900/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3AE2BEC7-1318-E24A-821B-0CDF78D20C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0741D1-B961-E74E-AA87-69279EE16571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16400" xr2:uid="{003416CE-73FF-424E-B43B-38F83879EA9F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
   <si>
     <t>Date</t>
   </si>
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AC8E64-8D22-B347-9054-4B5EE4E66514}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -462,6 +462,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>45183</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Task: Completed daily operations, 8 hours, 09/15
</commit_message>
<xml_diff>
--- a/CISC 4900 - Time Log Spreadsheet.xlsx
+++ b/CISC 4900 - Time Log Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicole/Documents/GitHub/CISC4900/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0741D1-B961-E74E-AA87-69279EE16571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77201C4F-DCFE-A94C-8D61-63F45081B8A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16400" xr2:uid="{003416CE-73FF-424E-B43B-38F83879EA9F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="5">
   <si>
     <t>Date</t>
   </si>
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AC8E64-8D22-B347-9054-4B5EE4E66514}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -473,6 +473,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>45184</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Task: Completed daily operations, 8 hours, 09/21
</commit_message>
<xml_diff>
--- a/CISC 4900 - Time Log Spreadsheet.xlsx
+++ b/CISC 4900 - Time Log Spreadsheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicole/Documents/GitHub/CISC4900/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DEADAC9-3DBA-F445-BEBB-367373E1B500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{357EE7D8-72E0-214F-8A5E-B811368F2B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16400" xr2:uid="{003416CE-73FF-424E-B43B-38F83879EA9F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="5">
   <si>
     <t>Date</t>
   </si>
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AC8E64-8D22-B347-9054-4B5EE4E66514}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -484,6 +484,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>45190</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Task: Completed daily operations, 8 hours, 09/22
</commit_message>
<xml_diff>
--- a/CISC 4900 - Time Log Spreadsheet.xlsx
+++ b/CISC 4900 - Time Log Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicole/Documents/GitHub/CISC4900/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{357EE7D8-72E0-214F-8A5E-B811368F2B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63C3B8C-2C82-7941-8ADD-7265C6734E49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16400" xr2:uid="{003416CE-73FF-424E-B43B-38F83879EA9F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="5">
   <si>
     <t>Date</t>
   </si>
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AC8E64-8D22-B347-9054-4B5EE4E66514}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -495,6 +495,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>45191</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Task: Completed daily operations, 8 hours, 09/28
</commit_message>
<xml_diff>
--- a/CISC 4900 - Time Log Spreadsheet.xlsx
+++ b/CISC 4900 - Time Log Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicole/Documents/GitHub/CISC4900/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63C3B8C-2C82-7941-8ADD-7265C6734E49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6C19E0-7602-A143-8727-B4CC94A1AEC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16400" xr2:uid="{003416CE-73FF-424E-B43B-38F83879EA9F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="5">
   <si>
     <t>Date</t>
   </si>
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AC8E64-8D22-B347-9054-4B5EE4E66514}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -506,6 +506,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>45197</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Task: Completed daily operations, 8 hours, 09/29
</commit_message>
<xml_diff>
--- a/CISC 4900 - Time Log Spreadsheet.xlsx
+++ b/CISC 4900 - Time Log Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicole/Documents/GitHub/CISC4900/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6C19E0-7602-A143-8727-B4CC94A1AEC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D8A7E7-8268-F746-B143-E4373A2D8EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16400" xr2:uid="{003416CE-73FF-424E-B43B-38F83879EA9F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="5">
   <si>
     <t>Date</t>
   </si>
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AC8E64-8D22-B347-9054-4B5EE4E66514}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -517,6 +517,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>45198</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Task: Completed daily operations, 8 hours, 10/05
</commit_message>
<xml_diff>
--- a/CISC 4900 - Time Log Spreadsheet.xlsx
+++ b/CISC 4900 - Time Log Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicole/Documents/GitHub/CISC4900/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D8A7E7-8268-F746-B143-E4373A2D8EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09F3784-0E7E-984D-BFD0-519A6B1D6E19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16400" xr2:uid="{003416CE-73FF-424E-B43B-38F83879EA9F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Completed 8 hours assisting with daily operations</t>
+  </si>
+  <si>
+    <t>Contributed technical work by aiding in resolving inconsistencies flagged by the system for employee calls</t>
   </si>
 </sst>
 </file>
@@ -416,7 +419,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AC8E64-8D22-B347-9054-4B5EE4E66514}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
@@ -426,7 +429,7 @@
   <cols>
     <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="2" max="2" width="18.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="54.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="108.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -528,6 +531,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>45204</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Task: Completed daily operations, 8 hours, 10/06
</commit_message>
<xml_diff>
--- a/CISC 4900 - Time Log Spreadsheet.xlsx
+++ b/CISC 4900 - Time Log Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicole/Documents/GitHub/CISC4900/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09F3784-0E7E-984D-BFD0-519A6B1D6E19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B4499C-3DFA-F942-97F0-7BCF32BB924E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16400" xr2:uid="{003416CE-73FF-424E-B43B-38F83879EA9F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AC8E64-8D22-B347-9054-4B5EE4E66514}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -542,6 +542,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>45205</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Task: Completed daily operations, 8 hours, 10/12
</commit_message>
<xml_diff>
--- a/CISC 4900 - Time Log Spreadsheet.xlsx
+++ b/CISC 4900 - Time Log Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicole/Documents/GitHub/CISC4900/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B4499C-3DFA-F942-97F0-7BCF32BB924E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35808F20-689D-624E-824B-5520A1E42036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16400" xr2:uid="{003416CE-73FF-424E-B43B-38F83879EA9F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AC8E64-8D22-B347-9054-4B5EE4E66514}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -553,6 +553,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>45211</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
sx Task: Completed daily operations, 8 hours, 10/13
</commit_message>
<xml_diff>
--- a/CISC 4900 - Time Log Spreadsheet.xlsx
+++ b/CISC 4900 - Time Log Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicole/Documents/GitHub/CISC4900/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35808F20-689D-624E-824B-5520A1E42036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A309FF-D4E9-F245-AFD4-69F1837B653A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16400" xr2:uid="{003416CE-73FF-424E-B43B-38F83879EA9F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AC8E64-8D22-B347-9054-4B5EE4E66514}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -564,6 +564,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>45212</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Task: Completed daily operations, 8 hours, 10/19
</commit_message>
<xml_diff>
--- a/CISC 4900 - Time Log Spreadsheet.xlsx
+++ b/CISC 4900 - Time Log Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicole/Documents/GitHub/CISC4900/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A309FF-D4E9-F245-AFD4-69F1837B653A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B8CDDB-DA6D-D441-BB22-C5866A16851A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16400" xr2:uid="{003416CE-73FF-424E-B43B-38F83879EA9F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AC8E64-8D22-B347-9054-4B5EE4E66514}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -575,6 +575,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>45218</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Task: Completed daily operations, 8 hours, 10/20
</commit_message>
<xml_diff>
--- a/CISC 4900 - Time Log Spreadsheet.xlsx
+++ b/CISC 4900 - Time Log Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicole/Documents/GitHub/CISC4900/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B8CDDB-DA6D-D441-BB22-C5866A16851A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63ADD0E-A758-2446-9BB7-FCBBCA275D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16400" xr2:uid="{003416CE-73FF-424E-B43B-38F83879EA9F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AC8E64-8D22-B347-9054-4B5EE4E66514}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -586,6 +586,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>45219</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Task: Completed daily operations, 8 hours, 10/26
</commit_message>
<xml_diff>
--- a/CISC 4900 - Time Log Spreadsheet.xlsx
+++ b/CISC 4900 - Time Log Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicole/Documents/GitHub/CISC4900/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63ADD0E-A758-2446-9BB7-FCBBCA275D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A12B1BF-0A36-4340-AF14-B7CCB323DA57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16400" xr2:uid="{003416CE-73FF-424E-B43B-38F83879EA9F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AC8E64-8D22-B347-9054-4B5EE4E66514}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -597,6 +597,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>45225</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Task: Completed daily operations, 8 hours, 10/27
</commit_message>
<xml_diff>
--- a/CISC 4900 - Time Log Spreadsheet.xlsx
+++ b/CISC 4900 - Time Log Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicole/Documents/GitHub/CISC4900/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A12B1BF-0A36-4340-AF14-B7CCB323DA57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531F2FD2-8F4B-3047-8E59-573B82857252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16400" xr2:uid="{003416CE-73FF-424E-B43B-38F83879EA9F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AC8E64-8D22-B347-9054-4B5EE4E66514}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -608,6 +608,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>45226</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Task: Completed daily operations, 8 hours, 11/02
</commit_message>
<xml_diff>
--- a/CISC 4900 - Time Log Spreadsheet.xlsx
+++ b/CISC 4900 - Time Log Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicole/Documents/GitHub/CISC4900/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531F2FD2-8F4B-3047-8E59-573B82857252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850DB0C8-DD88-3A48-B0AF-DD31274F1F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16400" xr2:uid="{003416CE-73FF-424E-B43B-38F83879EA9F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AC8E64-8D22-B347-9054-4B5EE4E66514}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -619,6 +619,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>45232</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Task: Completed daily operations, 8 hours, 11/03
</commit_message>
<xml_diff>
--- a/CISC 4900 - Time Log Spreadsheet.xlsx
+++ b/CISC 4900 - Time Log Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicole/Documents/GitHub/CISC4900/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850DB0C8-DD88-3A48-B0AF-DD31274F1F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED76A3C-6E56-4044-A869-0BD38E421B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16400" xr2:uid="{003416CE-73FF-424E-B43B-38F83879EA9F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AC8E64-8D22-B347-9054-4B5EE4E66514}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -630,6 +630,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>45233</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Task: Completed daily operations, 8 hours, 11/09
</commit_message>
<xml_diff>
--- a/CISC 4900 - Time Log Spreadsheet.xlsx
+++ b/CISC 4900 - Time Log Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicole/Documents/GitHub/CISC4900/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED76A3C-6E56-4044-A869-0BD38E421B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC87A19C-6ADC-AE43-9C26-EB3500755223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16400" xr2:uid="{003416CE-73FF-424E-B43B-38F83879EA9F}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16360" xr2:uid="{003416CE-73FF-424E-B43B-38F83879EA9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AC8E64-8D22-B347-9054-4B5EE4E66514}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -641,6 +641,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>45239</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Task: Completed daily operations, 8 hours, 11/10
</commit_message>
<xml_diff>
--- a/CISC 4900 - Time Log Spreadsheet.xlsx
+++ b/CISC 4900 - Time Log Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicole/Documents/GitHub/CISC4900/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC87A19C-6ADC-AE43-9C26-EB3500755223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD45FE18-46B1-4C45-942A-3B3725B54A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16360" xr2:uid="{003416CE-73FF-424E-B43B-38F83879EA9F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AC8E64-8D22-B347-9054-4B5EE4E66514}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -652,6 +652,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>45240</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Task: Completed daily operations, 8 hours, 11/16
</commit_message>
<xml_diff>
--- a/CISC 4900 - Time Log Spreadsheet.xlsx
+++ b/CISC 4900 - Time Log Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicole/Documents/GitHub/CISC4900/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD45FE18-46B1-4C45-942A-3B3725B54A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4CAE84-CB37-0B41-828A-1FC59C9B2E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16360" xr2:uid="{003416CE-73FF-424E-B43B-38F83879EA9F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AC8E64-8D22-B347-9054-4B5EE4E66514}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -663,6 +663,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>45246</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Task: Completed daily operations, 8 hours, 11/17
</commit_message>
<xml_diff>
--- a/CISC 4900 - Time Log Spreadsheet.xlsx
+++ b/CISC 4900 - Time Log Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicole/Documents/GitHub/CISC4900/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4CAE84-CB37-0B41-828A-1FC59C9B2E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0BBD5B-FEBA-2F44-B2FA-400E97010957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16360" xr2:uid="{003416CE-73FF-424E-B43B-38F83879EA9F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AC8E64-8D22-B347-9054-4B5EE4E66514}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -674,6 +674,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>45247</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Task: Completed daily operations, 8 hours, 11/24
</commit_message>
<xml_diff>
--- a/CISC 4900 - Time Log Spreadsheet.xlsx
+++ b/CISC 4900 - Time Log Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicole/Documents/GitHub/CISC4900/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0BBD5B-FEBA-2F44-B2FA-400E97010957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15564CA7-0D94-AD44-8A4D-EC1112971BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16360" xr2:uid="{003416CE-73FF-424E-B43B-38F83879EA9F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AC8E64-8D22-B347-9054-4B5EE4E66514}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -685,6 +685,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>45254</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Task: Completed daily operations, 8 hours, 11/30
</commit_message>
<xml_diff>
--- a/CISC 4900 - Time Log Spreadsheet.xlsx
+++ b/CISC 4900 - Time Log Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicole/Documents/GitHub/CISC4900/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15564CA7-0D94-AD44-8A4D-EC1112971BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A35F5C-6692-A44B-AA29-4CA3E5446E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16360" xr2:uid="{003416CE-73FF-424E-B43B-38F83879EA9F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AC8E64-8D22-B347-9054-4B5EE4E66514}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -696,6 +696,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>45260</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Task: Completed daily operations, 8 hours, 12/01
</commit_message>
<xml_diff>
--- a/CISC 4900 - Time Log Spreadsheet.xlsx
+++ b/CISC 4900 - Time Log Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicole/Documents/GitHub/CISC4900/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A35F5C-6692-A44B-AA29-4CA3E5446E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C85FD2-1BA8-3E4D-B6D4-6E13A18C5E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16360" xr2:uid="{003416CE-73FF-424E-B43B-38F83879EA9F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AC8E64-8D22-B347-9054-4B5EE4E66514}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -707,6 +707,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>45261</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Task: Completed daily operations, 8 hours, 12/07
</commit_message>
<xml_diff>
--- a/CISC 4900 - Time Log Spreadsheet.xlsx
+++ b/CISC 4900 - Time Log Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicole/Documents/GitHub/CISC4900/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C85FD2-1BA8-3E4D-B6D4-6E13A18C5E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2689897C-A488-FF44-906D-F3E02AAB9AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16360" xr2:uid="{003416CE-73FF-424E-B43B-38F83879EA9F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AC8E64-8D22-B347-9054-4B5EE4E66514}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -718,6 +718,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>45267</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Task: Completed daily operations, 8 hours, 12/08
</commit_message>
<xml_diff>
--- a/CISC 4900 - Time Log Spreadsheet.xlsx
+++ b/CISC 4900 - Time Log Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicole/Documents/GitHub/CISC4900/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2689897C-A488-FF44-906D-F3E02AAB9AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1055BCF2-A0B4-1442-A668-4EE831A6A1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16360" xr2:uid="{003416CE-73FF-424E-B43B-38F83879EA9F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AC8E64-8D22-B347-9054-4B5EE4E66514}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -729,6 +729,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>45268</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>